<commit_message>
Nova alterações, criando de tabelas pra agrupar os grupos de cada combinacao
</commit_message>
<xml_diff>
--- a/lotofacil.xlsx
+++ b/lotofacil.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="25455" windowHeight="10980" tabRatio="500" activeTab="5"/>
+    <workbookView windowWidth="25455" windowHeight="10980" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="HORIZONTAL" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="DIAGONAL" sheetId="4" r:id="rId4"/>
     <sheet name="NOVOS_REPETIDOS" sheetId="5" r:id="rId5"/>
     <sheet name="PAR_IMPAR" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -117,10 +118,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -158,6 +159,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -165,26 +167,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -197,35 +183,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,17 +205,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -261,9 +246,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,14 +278,15 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -305,6 +298,14 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="46">
     <fill>
@@ -315,6 +316,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -322,12 +329,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,181 +400,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,6 +599,17 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -635,13 +647,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -661,21 +677,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -689,143 +690,146 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -834,40 +838,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1291,111 +1283,111 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="6" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1025" width="9.14285714285714" style="11" customWidth="1"/>
+    <col min="1" max="1025" width="9.14285714285714" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="2">
         <v>3</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="2">
         <v>4</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="2">
         <v>6</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="2">
         <v>7</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="2">
         <v>8</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="2">
         <v>9</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="2">
         <v>11</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="2">
         <v>12</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="2">
         <v>13</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="2">
         <v>14</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="2">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="2">
         <v>16</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="2">
         <v>17</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="2">
         <v>18</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="2">
         <v>19</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="2">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="2">
         <v>21</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="2">
         <v>22</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="2">
         <v>23</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="2">
         <v>24</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="2">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
@@ -1433,97 +1425,97 @@
       </c>
     </row>
     <row r="3" spans="3:8">
-      <c r="C3" s="11"/>
-      <c r="D3" s="20">
+      <c r="C3" s="2"/>
+      <c r="D3" s="17">
         <v>1</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="20">
         <v>2</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="19">
         <v>3</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="16">
         <v>4</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="21">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="3:8">
-      <c r="C4" s="11"/>
-      <c r="D4" s="20">
+      <c r="C4" s="2"/>
+      <c r="D4" s="17">
         <v>6</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="20">
         <v>7</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="19">
         <v>8</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="16">
         <v>9</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="21">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="3:8">
-      <c r="C5" s="11"/>
-      <c r="D5" s="20">
+      <c r="C5" s="2"/>
+      <c r="D5" s="17">
         <v>11</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="20">
         <v>12</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="19">
         <v>13</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="16">
         <v>14</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="21">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="3:8">
-      <c r="C6" s="11"/>
-      <c r="D6" s="20">
+      <c r="C6" s="2"/>
+      <c r="D6" s="17">
         <v>16</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="20">
         <v>17</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="19">
         <v>18</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="16">
         <v>19</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="21">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="3:8">
-      <c r="C7" s="11"/>
-      <c r="D7" s="20">
+      <c r="C7" s="2"/>
+      <c r="D7" s="17">
         <v>21</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="20">
         <v>22</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="19">
         <v>23</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="16">
         <v>24</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="21">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
@@ -1544,92 +1536,92 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:8">
-      <c r="D3" s="20">
+      <c r="D3" s="17">
         <v>1</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="17">
         <v>2</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="18">
         <v>3</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="16">
         <v>4</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="4:8">
-      <c r="D4" s="20">
+      <c r="D4" s="17">
         <v>6</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="17">
         <v>7</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="18">
         <v>8</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="16">
         <v>9</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="16">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="4:8">
-      <c r="D5" s="20">
+      <c r="D5" s="17">
         <v>11</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="15">
         <v>12</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="18">
         <v>13</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="19">
         <v>14</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="16">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="4:8">
-      <c r="D6" s="18">
+      <c r="D6" s="15">
         <v>16</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="15">
         <v>17</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="18">
         <v>18</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="19">
         <v>19</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="19">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="4:8">
-      <c r="D7" s="18">
+      <c r="D7" s="15">
         <v>21</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="15">
         <v>22</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="18">
         <v>23</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="19">
         <v>24</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="19">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
@@ -1646,96 +1638,96 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="6" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1025" width="9.14285714285714" style="11" customWidth="1"/>
+    <col min="1" max="1025" width="9.14285714285714" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="4:8">
-      <c r="D3" s="16">
+      <c r="D3" s="13">
         <v>1</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="17">
         <v>2</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="16">
         <v>3</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="15">
         <v>4</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="14">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="4:8">
-      <c r="D4" s="17">
+      <c r="D4" s="14">
         <v>6</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="13">
         <v>7</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="17">
         <v>8</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="16">
         <v>9</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="15">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="4:8">
-      <c r="D5" s="18">
+      <c r="D5" s="15">
         <v>11</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="14">
         <v>12</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="13">
         <v>13</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="17">
         <v>14</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="16">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="4:8">
-      <c r="D6" s="19">
+      <c r="D6" s="16">
         <v>16</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="15">
         <v>17</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="14">
         <v>18</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="13">
         <v>19</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="17">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="4:8">
-      <c r="D7" s="20">
+      <c r="D7" s="17">
         <v>21</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="16">
         <v>22</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="15">
         <v>23</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="14">
         <v>24</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="13">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
@@ -1752,214 +1744,214 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="4" width="11.5238095238095" style="11"/>
-    <col min="5" max="5" width="8.14285714285714" style="11" customWidth="1"/>
-    <col min="6" max="6" width="11.2857142857143" style="11" customWidth="1"/>
-    <col min="7" max="7" width="17.4285714285714" style="11" customWidth="1"/>
-    <col min="8" max="8" width="16.1428571428571" style="11" customWidth="1"/>
-    <col min="9" max="9" width="58" style="11" customWidth="1"/>
-    <col min="10" max="10" width="11.5238095238095" style="11"/>
-    <col min="11" max="11" width="17.4285714285714" style="11" customWidth="1"/>
-    <col min="12" max="12" width="10.5714285714286" style="11" customWidth="1"/>
-    <col min="13" max="13" width="10.2857142857143" style="11" customWidth="1"/>
-    <col min="14" max="1027" width="11.5238095238095" style="11"/>
+    <col min="1" max="4" width="11.5238095238095" style="2"/>
+    <col min="5" max="5" width="8.14285714285714" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.2857142857143" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.4285714285714" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.1428571428571" style="2" customWidth="1"/>
+    <col min="9" max="9" width="58" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.5238095238095" style="2"/>
+    <col min="11" max="11" width="17.4285714285714" style="2" customWidth="1"/>
+    <col min="12" max="12" width="10.5714285714286" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.2857142857143" style="2" customWidth="1"/>
+    <col min="14" max="1027" width="11.5238095238095" style="2"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:7">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="2:13">
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="L7" s="13" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="L7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="13"/>
+      <c r="M7" s="11"/>
     </row>
     <row r="8" spans="12:13">
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="M8" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="5:13">
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="11" t="s">
+      <c r="L9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="11" t="s">
+      <c r="M9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" ht="25.5" spans="5:13">
-      <c r="E10" s="11">
+      <c r="E10" s="2">
         <v>0</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="2">
         <v>15</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="2">
         <v>0</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="2">
         <v>0</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="L10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="M10" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="5:13">
-      <c r="E11" s="11">
+      <c r="E11" s="2">
         <v>1</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="2">
         <v>14</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="L11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="M11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="5:13">
-      <c r="E12" s="11">
+      <c r="E12" s="2">
         <v>2</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="2">
         <v>13</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="11" t="s">
+      <c r="L12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M12" s="11" t="s">
+      <c r="M12" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="5:6">
-      <c r="E13" s="11">
+      <c r="E13" s="2">
         <v>3</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="5:6">
-      <c r="E14" s="11">
+      <c r="E14" s="2">
         <v>4</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="2">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="5:6">
-      <c r="E15" s="11">
+      <c r="E15" s="2">
         <v>5</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="5:6">
-      <c r="E16" s="11">
+      <c r="E16" s="2">
         <v>6</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="2">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="5:6">
-      <c r="E17" s="11">
+      <c r="E17" s="2">
         <v>7</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="2">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="5:6">
-      <c r="E18" s="11">
+      <c r="E18" s="2">
         <v>8</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="5:6">
-      <c r="E19" s="11">
+      <c r="E19" s="2">
         <v>9</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="5:6">
-      <c r="E20" s="11">
+      <c r="E20" s="2">
         <v>10</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="2">
         <v>5</v>
       </c>
     </row>
@@ -1985,36 +1977,36 @@
   <sheetPr/>
   <dimension ref="A3:R37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="12" width="9.14285714285714" style="1"/>
-    <col min="13" max="13" width="13.8571428571429" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.14285714285714" style="1"/>
+    <col min="1" max="12" width="9.14285714285714" style="2"/>
+    <col min="13" max="13" width="13.8571428571429" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="9.14285714285714" style="2"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:18">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
     </row>
     <row r="6" spans="9:12">
       <c r="I6" s="9" t="s">
@@ -2025,16 +2017,16 @@
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="2:13">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="4" t="s">
         <v>28</v>
       </c>
       <c r="I7" s="10">
@@ -2049,12 +2041,12 @@
       <c r="L7" s="10">
         <v>18</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="3:12">
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="6">
@@ -2063,28 +2055,28 @@
       <c r="H8" s="6">
         <v>13</v>
       </c>
-      <c r="I8" s="1" t="str">
+      <c r="I8" s="2" t="str">
         <f t="shared" ref="I8:L8" si="0">IF(SUM($G8:$H8)=I$7,"X","")</f>
         <v>X</v>
       </c>
-      <c r="J8" s="1" t="str">
+      <c r="J8" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K8" s="1" t="str">
+      <c r="K8" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="L8" s="1" t="str">
+      <c r="L8" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>2</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>3</v>
       </c>
       <c r="G9" s="6">
@@ -2093,28 +2085,28 @@
       <c r="H9" s="6">
         <v>12</v>
       </c>
-      <c r="I9" s="1" t="str">
+      <c r="I9" s="2" t="str">
         <f t="shared" ref="I9:I37" si="1">IF(SUM($G9:$H9)=I$7,"X","")</f>
         <v>X</v>
       </c>
-      <c r="J9" s="1" t="str">
+      <c r="J9" s="2" t="str">
         <f t="shared" ref="J9:J37" si="2">IF(SUM($G9:$H9)=J$7,"X","")</f>
         <v/>
       </c>
-      <c r="K9" s="1" t="str">
+      <c r="K9" s="2" t="str">
         <f t="shared" ref="K9:K37" si="3">IF(SUM($G9:$H9)=K$7,"X","")</f>
         <v/>
       </c>
-      <c r="L9" s="1" t="str">
+      <c r="L9" s="2" t="str">
         <f t="shared" ref="L9:L37" si="4">IF(SUM($G9:$H9)=L$7,"X","")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="2:12">
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>4</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>5</v>
       </c>
       <c r="G10" s="6">
@@ -2123,28 +2115,28 @@
       <c r="H10" s="6">
         <v>11</v>
       </c>
-      <c r="I10" s="1" t="str">
+      <c r="I10" s="2" t="str">
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="J10" s="1" t="str">
+      <c r="J10" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K10" s="1" t="str">
+      <c r="K10" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L10" s="1" t="str">
+      <c r="L10" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="11" spans="2:12">
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>6</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>7</v>
       </c>
       <c r="G11" s="6">
@@ -2153,28 +2145,28 @@
       <c r="H11" s="6">
         <v>10</v>
       </c>
-      <c r="I11" s="1" t="str">
+      <c r="I11" s="2" t="str">
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="J11" s="1" t="str">
+      <c r="J11" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K11" s="1" t="str">
+      <c r="K11" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L11" s="1" t="str">
+      <c r="L11" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>8</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>9</v>
       </c>
       <c r="G12" s="6">
@@ -2183,28 +2175,28 @@
       <c r="H12" s="6">
         <v>9</v>
       </c>
-      <c r="I12" s="1" t="str">
+      <c r="I12" s="2" t="str">
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="J12" s="1" t="str">
+      <c r="J12" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K12" s="1" t="str">
+      <c r="K12" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L12" s="1" t="str">
+      <c r="L12" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="13" spans="2:12">
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>10</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>11</v>
       </c>
       <c r="G13" s="6">
@@ -2213,28 +2205,28 @@
       <c r="H13" s="6">
         <v>8</v>
       </c>
-      <c r="I13" s="1" t="str">
+      <c r="I13" s="2" t="str">
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="J13" s="1" t="str">
+      <c r="J13" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K13" s="1" t="str">
+      <c r="K13" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L13" s="1" t="str">
+      <c r="L13" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="14" spans="2:12">
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>12</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="2">
         <v>13</v>
       </c>
       <c r="G14" s="6">
@@ -2243,28 +2235,28 @@
       <c r="H14" s="6">
         <v>7</v>
       </c>
-      <c r="I14" s="1" t="str">
+      <c r="I14" s="2" t="str">
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="J14" s="1" t="str">
+      <c r="J14" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K14" s="1" t="str">
+      <c r="K14" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L14" s="1" t="str">
+      <c r="L14" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>14</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>15</v>
       </c>
       <c r="G15" s="6">
@@ -2273,28 +2265,28 @@
       <c r="H15" s="6">
         <v>6</v>
       </c>
-      <c r="I15" s="1" t="str">
+      <c r="I15" s="2" t="str">
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="J15" s="1" t="str">
+      <c r="J15" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K15" s="1" t="str">
+      <c r="K15" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L15" s="1" t="str">
+      <c r="L15" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>16</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <v>17</v>
       </c>
       <c r="G16" s="6">
@@ -2303,28 +2295,28 @@
       <c r="H16" s="6">
         <v>5</v>
       </c>
-      <c r="I16" s="1" t="str">
+      <c r="I16" s="2" t="str">
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="J16" s="1" t="str">
+      <c r="J16" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K16" s="1" t="str">
+      <c r="K16" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L16" s="1" t="str">
+      <c r="L16" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="2:12">
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>18</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="2">
         <v>19</v>
       </c>
       <c r="G17" s="6">
@@ -2333,28 +2325,28 @@
       <c r="H17" s="6">
         <v>4</v>
       </c>
-      <c r="I17" s="1" t="str">
+      <c r="I17" s="2" t="str">
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="J17" s="1" t="str">
+      <c r="J17" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K17" s="1" t="str">
+      <c r="K17" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L17" s="1" t="str">
+      <c r="L17" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="2:12">
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>20</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <v>21</v>
       </c>
       <c r="G18" s="6">
@@ -2363,28 +2355,28 @@
       <c r="H18" s="6">
         <v>3</v>
       </c>
-      <c r="I18" s="1" t="str">
+      <c r="I18" s="2" t="str">
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="J18" s="1" t="str">
+      <c r="J18" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K18" s="1" t="str">
+      <c r="K18" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L18" s="1" t="str">
+      <c r="L18" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="2:12">
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>22</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="2">
         <v>23</v>
       </c>
       <c r="G19" s="7">
@@ -2393,28 +2385,28 @@
       <c r="H19" s="7">
         <v>13</v>
       </c>
-      <c r="I19" s="1" t="str">
+      <c r="I19" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J19" s="1" t="str">
+      <c r="J19" s="2" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="K19" s="1" t="str">
+      <c r="K19" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L19" s="1" t="str">
+      <c r="L19" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="2:12">
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>24</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="2">
         <v>25</v>
       </c>
       <c r="G20" s="7">
@@ -2423,25 +2415,25 @@
       <c r="H20" s="7">
         <v>12</v>
       </c>
-      <c r="I20" s="1" t="str">
+      <c r="I20" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J20" s="1" t="str">
+      <c r="J20" s="2" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="K20" s="1" t="str">
+      <c r="K20" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L20" s="1" t="str">
+      <c r="L20" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="5">
@@ -2458,19 +2450,19 @@
       <c r="H21" s="7">
         <v>11</v>
       </c>
-      <c r="I21" s="1" t="str">
+      <c r="I21" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J21" s="1" t="str">
+      <c r="J21" s="2" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="K21" s="1" t="str">
+      <c r="K21" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L21" s="1" t="str">
+      <c r="L21" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2482,19 +2474,19 @@
       <c r="H22" s="7">
         <v>10</v>
       </c>
-      <c r="I22" s="1" t="str">
+      <c r="I22" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J22" s="1" t="str">
+      <c r="J22" s="2" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="K22" s="1" t="str">
+      <c r="K22" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L22" s="1" t="str">
+      <c r="L22" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2506,19 +2498,19 @@
       <c r="H23" s="7">
         <v>9</v>
       </c>
-      <c r="I23" s="1" t="str">
+      <c r="I23" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J23" s="1" t="str">
+      <c r="J23" s="2" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="K23" s="1" t="str">
+      <c r="K23" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L23" s="1" t="str">
+      <c r="L23" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2530,19 +2522,19 @@
       <c r="H24" s="7">
         <v>8</v>
       </c>
-      <c r="I24" s="1" t="str">
+      <c r="I24" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J24" s="1" t="str">
+      <c r="J24" s="2" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="K24" s="1" t="str">
+      <c r="K24" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L24" s="1" t="str">
+      <c r="L24" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2554,19 +2546,19 @@
       <c r="H25" s="7">
         <v>7</v>
       </c>
-      <c r="I25" s="1" t="str">
+      <c r="I25" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J25" s="1" t="str">
+      <c r="J25" s="2" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="K25" s="1" t="str">
+      <c r="K25" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L25" s="1" t="str">
+      <c r="L25" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2578,19 +2570,19 @@
       <c r="H26" s="7">
         <v>6</v>
       </c>
-      <c r="I26" s="1" t="str">
+      <c r="I26" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J26" s="1" t="str">
+      <c r="J26" s="2" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="K26" s="1" t="str">
+      <c r="K26" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L26" s="1" t="str">
+      <c r="L26" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2602,19 +2594,19 @@
       <c r="H27" s="7">
         <v>5</v>
       </c>
-      <c r="I27" s="1" t="str">
+      <c r="I27" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J27" s="1" t="str">
+      <c r="J27" s="2" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="K27" s="1" t="str">
+      <c r="K27" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L27" s="1" t="str">
+      <c r="L27" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2626,19 +2618,19 @@
       <c r="H28" s="7">
         <v>4</v>
       </c>
-      <c r="I28" s="1" t="str">
+      <c r="I28" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J28" s="1" t="str">
+      <c r="J28" s="2" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="K28" s="1" t="str">
+      <c r="K28" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L28" s="1" t="str">
+      <c r="L28" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2650,19 +2642,19 @@
       <c r="H29" s="8">
         <v>13</v>
       </c>
-      <c r="I29" s="1" t="str">
+      <c r="I29" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J29" s="1" t="str">
+      <c r="J29" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K29" s="1" t="str">
+      <c r="K29" s="2" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="L29" s="1" t="str">
+      <c r="L29" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2674,19 +2666,19 @@
       <c r="H30" s="8">
         <v>12</v>
       </c>
-      <c r="I30" s="1" t="str">
+      <c r="I30" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J30" s="1" t="str">
+      <c r="J30" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K30" s="1" t="str">
+      <c r="K30" s="2" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="L30" s="1" t="str">
+      <c r="L30" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2698,19 +2690,19 @@
       <c r="H31" s="8">
         <v>11</v>
       </c>
-      <c r="I31" s="1" t="str">
+      <c r="I31" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J31" s="1" t="str">
+      <c r="J31" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K31" s="1" t="str">
+      <c r="K31" s="2" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="L31" s="1" t="str">
+      <c r="L31" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2722,19 +2714,19 @@
       <c r="H32" s="8">
         <v>10</v>
       </c>
-      <c r="I32" s="1" t="str">
+      <c r="I32" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J32" s="1" t="str">
+      <c r="J32" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K32" s="1" t="str">
+      <c r="K32" s="2" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="L32" s="1" t="str">
+      <c r="L32" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2746,19 +2738,19 @@
       <c r="H33" s="8">
         <v>9</v>
       </c>
-      <c r="I33" s="1" t="str">
+      <c r="I33" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J33" s="1" t="str">
+      <c r="J33" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K33" s="1" t="str">
+      <c r="K33" s="2" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="L33" s="1" t="str">
+      <c r="L33" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2770,19 +2762,19 @@
       <c r="H34" s="8">
         <v>8</v>
       </c>
-      <c r="I34" s="1" t="str">
+      <c r="I34" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J34" s="1" t="str">
+      <c r="J34" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K34" s="1" t="str">
+      <c r="K34" s="2" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="L34" s="1" t="str">
+      <c r="L34" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2794,19 +2786,19 @@
       <c r="H35" s="8">
         <v>7</v>
       </c>
-      <c r="I35" s="1" t="str">
+      <c r="I35" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J35" s="1" t="str">
+      <c r="J35" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K35" s="1" t="str">
+      <c r="K35" s="2" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="L35" s="1" t="str">
+      <c r="L35" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2818,19 +2810,19 @@
       <c r="H36" s="8">
         <v>6</v>
       </c>
-      <c r="I36" s="1" t="str">
+      <c r="I36" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J36" s="1" t="str">
+      <c r="J36" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K36" s="1" t="str">
+      <c r="K36" s="2" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="L36" s="1" t="str">
+      <c r="L36" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2842,19 +2834,19 @@
       <c r="H37" s="8">
         <v>5</v>
       </c>
-      <c r="I37" s="1" t="str">
+      <c r="I37" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J37" s="1" t="str">
+      <c r="J37" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K37" s="1" t="str">
+      <c r="K37" s="2" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="L37" s="1" t="str">
+      <c r="L37" s="2" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -2868,4 +2860,287 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="C3:T16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="3" max="11" width="2.57142857142857" customWidth="1"/>
+    <col min="12" max="17" width="3.57142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:17">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>8</v>
+      </c>
+      <c r="K3">
+        <v>9</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+      <c r="M3">
+        <v>11</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3">
+        <v>13</v>
+      </c>
+      <c r="P3">
+        <v>14</v>
+      </c>
+      <c r="Q3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="3:18">
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1">
+        <v>6</v>
+      </c>
+      <c r="I5" s="1">
+        <v>7</v>
+      </c>
+      <c r="J5" s="1">
+        <v>8</v>
+      </c>
+      <c r="K5" s="1">
+        <v>9</v>
+      </c>
+      <c r="L5" s="1">
+        <v>10</v>
+      </c>
+      <c r="M5" s="1">
+        <v>11</v>
+      </c>
+      <c r="N5" s="1">
+        <v>12</v>
+      </c>
+      <c r="O5" s="1">
+        <v>13</v>
+      </c>
+      <c r="P5">
+        <v>16</v>
+      </c>
+      <c r="Q5">
+        <v>17</v>
+      </c>
+      <c r="R5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="3:19">
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1">
+        <v>6</v>
+      </c>
+      <c r="I6" s="1">
+        <v>7</v>
+      </c>
+      <c r="J6" s="1">
+        <v>8</v>
+      </c>
+      <c r="K6" s="1">
+        <v>9</v>
+      </c>
+      <c r="L6" s="1">
+        <v>10</v>
+      </c>
+      <c r="M6" s="1">
+        <v>11</v>
+      </c>
+      <c r="N6" s="1">
+        <v>12</v>
+      </c>
+      <c r="O6" s="1">
+        <v>13</v>
+      </c>
+      <c r="P6">
+        <v>16</v>
+      </c>
+      <c r="Q6">
+        <v>17</v>
+      </c>
+      <c r="R6">
+        <v>18</v>
+      </c>
+      <c r="S6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="3:20">
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1">
+        <v>6</v>
+      </c>
+      <c r="I7" s="1">
+        <v>7</v>
+      </c>
+      <c r="J7" s="1">
+        <v>8</v>
+      </c>
+      <c r="K7" s="1">
+        <v>9</v>
+      </c>
+      <c r="L7" s="1">
+        <v>10</v>
+      </c>
+      <c r="M7" s="1">
+        <v>11</v>
+      </c>
+      <c r="N7" s="1">
+        <v>12</v>
+      </c>
+      <c r="O7" s="1">
+        <v>13</v>
+      </c>
+      <c r="P7">
+        <v>16</v>
+      </c>
+      <c r="Q7">
+        <v>17</v>
+      </c>
+      <c r="R7">
+        <v>18</v>
+      </c>
+      <c r="S7">
+        <v>19</v>
+      </c>
+      <c r="T7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="16:17">
+      <c r="P10">
+        <v>16</v>
+      </c>
+      <c r="Q10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="16:17">
+      <c r="P11">
+        <v>16</v>
+      </c>
+      <c r="Q11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="16:17">
+      <c r="P12">
+        <v>16</v>
+      </c>
+      <c r="Q12">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="16:17">
+      <c r="P13">
+        <v>16</v>
+      </c>
+      <c r="Q13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="16:17">
+      <c r="P14">
+        <v>16</v>
+      </c>
+      <c r="Q14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="16:17">
+      <c r="P15">
+        <v>17</v>
+      </c>
+      <c r="Q15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="16:17">
+      <c r="P16">
+        <v>17</v>
+      </c>
+      <c r="Q16">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>